<commit_message>
william russell rates update
</commit_message>
<xml_diff>
--- a/Inputs/William_russell/addons.xlsx
+++ b/Inputs/William_russell/addons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
   <si>
     <t xml:space="preserve">sheetName</t>
   </si>
@@ -96,16 +96,13 @@
     <t xml:space="preserve">Gold</t>
   </si>
   <si>
-    <t xml:space="preserve">planName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageStart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageEnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rates</t>
+    <t xml:space="preserve">minAge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxAge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -160,12 +157,48 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB85C00"/>
+        <bgColor rgb="FFEA7500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA7500"/>
+        <bgColor rgb="FFFF972F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF972F"/>
+        <bgColor rgb="FFFFB66C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFF972F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -209,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,7 +271,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,6 +308,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFFB66C"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFDBB6"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF972F"/>
+      <rgbColor rgb="FFEA7500"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFB85C00"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -262,10 +379,10 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
@@ -393,7 +510,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -409,26 +526,26 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,9 +562,9 @@
         <v>15</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>784.98</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>824.23</v>
+      </c>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -462,10 +579,10 @@
       <c r="D3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="n">
-        <v>1800.61073149117</v>
-      </c>
-      <c r="F3" s="7"/>
+      <c r="E3" s="9" t="n">
+        <v>1890.64</v>
+      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -480,10 +597,10 @@
       <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="n">
-        <v>2060.33</v>
-      </c>
-      <c r="F4" s="7"/>
+      <c r="E4" s="10" t="n">
+        <v>2163.35</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -498,10 +615,10 @@
       <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <v>2779.48</v>
-      </c>
-      <c r="F5" s="7"/>
+      <c r="E5" s="11" t="n">
+        <v>2918.45</v>
+      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -516,10 +633,10 @@
       <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7" t="n">
-        <v>3358.82</v>
-      </c>
-      <c r="F6" s="7"/>
+      <c r="E6" s="12" t="n">
+        <v>3526.76</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -534,12 +651,12 @@
       <c r="D7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="13" t="n">
         <v>3580.69</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -552,11 +669,11 @@
       <c r="D8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>1080.96</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="8" t="n">
+        <v>310.78</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -569,11 +686,11 @@
       <c r="D9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>2799.45073149117</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="8" t="n">
+        <v>1048.78</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -586,11 +703,11 @@
       <c r="D10" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>3199.01</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>1195.61</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -603,11 +720,11 @@
       <c r="D11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <v>4357.66</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="8" t="n">
+        <v>1657.09</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -620,11 +737,11 @@
       <c r="D12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>5855.93</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="8" t="n">
+        <v>2621.97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -637,8 +754,8 @@
       <c r="D13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <v>8375.08</v>
+      <c r="E13" s="8" t="n">
+        <v>5034.11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,8 +771,8 @@
       <c r="D14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="7" t="n">
-        <v>1104.98</v>
+      <c r="E14" s="8" t="n">
+        <v>1160.23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,8 +788,8 @@
       <c r="D15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="7" t="n">
-        <v>2477.1</v>
+      <c r="E15" s="8" t="n">
+        <v>2600.96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,8 +805,8 @@
       <c r="D16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="7" t="n">
-        <v>2956.53</v>
+      <c r="E16" s="8" t="n">
+        <v>3104.36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,8 +822,8 @@
       <c r="D17" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="7" t="n">
-        <v>4095.21</v>
+      <c r="E17" s="8" t="n">
+        <v>4299.97</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,8 +839,8 @@
       <c r="D18" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="7" t="n">
-        <v>6572.35</v>
+      <c r="E18" s="8" t="n">
+        <v>6900.97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,14 +856,14 @@
       <c r="D19" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="8" t="n">
         <v>7161.38</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -759,17 +876,108 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="n">
+        <v>784.98</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>1800.61073149117</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <v>2060.33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <v>2779.48</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>3358.82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>3580.69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1080.96</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2799.45073149117</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>3199.01</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4357.66</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5855.93</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>8375.08</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="n">
+        <v>1104.98</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="n">
+        <v>2477.1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="n">
+        <v>2956.53</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="n">
+        <v>4095.21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="n">
+        <v>6572.35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="n">
+        <v>7161.38</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>